<commit_message>
update to 2020 present year
</commit_message>
<xml_diff>
--- a/Arformoterol Input.xlsx
+++ b/Arformoterol Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgow\Documents\Clients\5. Vertice\Test outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1405D646-A88E-4CE6-9C78-B8C6AEAFDA6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4A232F-B7F6-443A-8CF1-D0A4D64FC4A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{717DFAA3-7B66-4F29-9F39-BAA921B8431C}"/>
   </bookViews>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E79D91C-6AD2-4213-9CA0-4A97474C00D8}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1464,7 +1464,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="45">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="57"/>
@@ -1924,51 +1924,51 @@
         <v>66</v>
       </c>
       <c r="B55" s="43">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C55" s="9">
         <f>B55+1</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D55" s="9">
         <f t="shared" ref="D55:M55" si="0">C55+1</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E55" s="9">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F55" s="9">
         <f t="shared" si="0"/>
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="G55" s="9">
         <f t="shared" si="0"/>
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="H55" s="9">
         <f t="shared" si="0"/>
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I55" s="9">
         <f t="shared" si="0"/>
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="J55" s="9">
         <f t="shared" si="0"/>
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="K55" s="9">
         <f t="shared" si="0"/>
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="L55" s="9">
         <f t="shared" si="0"/>
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="M55" s="9">
         <f t="shared" si="0"/>
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="N55" s="9" t="s">
         <v>121</v>

</xml_diff>